<commit_message>
Lavet en slags tidsplan over de forskellige faser vi dykker ind i.
</commit_message>
<xml_diff>
--- a/Tidsplan/Tidsplan.xlsx
+++ b/Tidsplan/Tidsplan.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -18,6 +18,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Opgaver/Ugenr</t>
+  </si>
+  <si>
+    <t>Projekt</t>
+  </si>
+  <si>
+    <t>Deadlines</t>
+  </si>
+  <si>
+    <t>Oprettelse af hold</t>
+  </si>
+  <si>
+    <t>Kravspec</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>Kravspec afleveres 16-02</t>
+  </si>
+  <si>
+    <t>Review 19-02 GRP5 + 21-02 GRP7</t>
+  </si>
+  <si>
+    <t>Analyse</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Implementering</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Aflevere projekt 30-05</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
@@ -29,15 +76,63 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +140,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +450,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+      <c r="D1">
+        <v>7</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>9</v>
+      </c>
+      <c r="G1">
+        <v>10</v>
+      </c>
+      <c r="H1">
+        <v>11</v>
+      </c>
+      <c r="I1">
+        <v>12</v>
+      </c>
+      <c r="J1">
+        <v>13</v>
+      </c>
+      <c r="K1">
+        <v>14</v>
+      </c>
+      <c r="L1">
+        <v>15</v>
+      </c>
+      <c r="M1">
+        <v>16</v>
+      </c>
+      <c r="N1">
+        <v>17</v>
+      </c>
+      <c r="O1">
+        <v>18</v>
+      </c>
+      <c r="P1">
+        <v>19</v>
+      </c>
+      <c r="Q1">
+        <v>20</v>
+      </c>
+      <c r="R1">
+        <v>21</v>
+      </c>
+      <c r="S1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="O7" s="8"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="R11" s="9"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ændret tidsplan til noget der passer til vores sprints.
</commit_message>
<xml_diff>
--- a/Tidsplan/Tidsplan.xlsx
+++ b/Tidsplan/Tidsplan.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tidsplan" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Opgaver/Ugenr</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Aflevere projekt 30-05</t>
+  </si>
+  <si>
+    <t>Opdeles i interne grupper</t>
   </si>
 </sst>
 </file>
@@ -76,7 +79,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,12 +107,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,16 +138,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -159,17 +150,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,6 +525,9 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -547,8 +543,26 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -559,14 +573,15 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -575,51 +590,56 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="O7" s="8"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="O7" s="7"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
       <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="R11" s="9"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="9"/>
+      <c r="R11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ændet Tidsplan.xlsx, nu er der ferie inkluderet
</commit_message>
<xml_diff>
--- a/Tidsplan/Tidsplan.xlsx
+++ b/Tidsplan/Tidsplan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Opgaver/Ugenr</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Opdeles i interne grupper</t>
+  </si>
+  <si>
+    <t>23-03 ferie</t>
   </si>
 </sst>
 </file>
@@ -445,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,6 +459,7 @@
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -538,6 +542,9 @@
       </c>
       <c r="E3" t="s">
         <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="S3" t="s">
         <v>13</v>
@@ -598,7 +605,8 @@
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="O7" s="7"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -615,8 +623,10 @@
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="6"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="6"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -624,19 +634,22 @@
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="4"/>
+      <c r="K10" s="9"/>
       <c r="L10" s="4"/>
-      <c r="Q10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="L11" s="9"/>
-      <c r="M11" s="8"/>
+      <c r="M11" s="9"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="9"/>
-      <c r="R11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tilføjet opdateret tidsplan med afleveringer til de fag vi har
</commit_message>
<xml_diff>
--- a/Tidsplan/Tidsplan.xlsx
+++ b/Tidsplan/Tidsplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27420" windowHeight="11100"/>
   </bookViews>
   <sheets>
     <sheet name="Tidsplan" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Opgaver/Ugenr</t>
   </si>
@@ -67,13 +67,38 @@
   </si>
   <si>
     <t>23-03 ferie</t>
+  </si>
+  <si>
+    <t>Afleveringer</t>
+  </si>
+  <si>
+    <t>16-04 SWD</t>
+  </si>
+  <si>
+    <t>15-04 SWT</t>
+  </si>
+  <si>
+    <t>15-05 IKN</t>
+  </si>
+  <si>
+    <t>25-04 SWT</t>
+  </si>
+  <si>
+    <t>27-04 DAB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +156,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -149,11 +179,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -166,8 +236,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="9" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bemærk!" xfId="1" builtinId="10"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,6 +535,9 @@
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -651,6 +729,47 @@
       <c r="R11" s="9"/>
       <c r="S11" s="8"/>
     </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>